<commit_message>
A simple example and a class to control X9C104 digipots
Fix typos

Fix typos

Fix typos
</commit_message>
<xml_diff>
--- a/x9cn0n/_more/x9c104-characteristics.xlsx
+++ b/x9cn0n/_more/x9c104-characteristics.xlsx
@@ -5,26 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krzysztof/esp/toit/x9c10n/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krzysztof/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDD08E1-70EC-8C49-B06F-DFAA26F62ACC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA7A06B-0903-924A-BDCE-60708608A4B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31000" yWindow="-13540" windowWidth="20960" windowHeight="15580" xr2:uid="{076B741B-539E-7A4E-A51B-F8F2665BE220}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$A$32</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$32</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$A$2:$A$32</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$2:$B$32</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,13 +30,13 @@
     <t>Step</t>
   </si>
   <si>
-    <t>Digipot A Resistancec [Ω]</t>
+    <t>Reference Resistance [Ω]</t>
   </si>
   <si>
-    <t>Digipot B Resistancec [Ω]</t>
+    <t>Digipot A Resistance [Ω]</t>
   </si>
   <si>
-    <t>Reference Resistance [Ω]</t>
+    <t>Digipot B Resistance [Ω]</t>
   </si>
 </sst>
 </file>
@@ -54,10 +44,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -85,10 +83,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -147,7 +146,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Digipot A Resistancec [Ω]</c:v>
+                  <c:v>Digipot A Resistance [Ω]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -394,7 +393,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Digipot B Resistancec [Ω]</c:v>
+                  <c:v>Digipot B Resistance [Ω]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1973,27 +1972,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE1272F-318E-3D4C-AB73-C1FC0D9B2526}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>